<commit_message>
update appointment and appointmentResponse
Built with canonical: http://example.org that has to be changed
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-no-basis-group.xlsx
+++ b/output/StructureDefinition-no-basis-group.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://hl7.no/fhir/structuredefinition/no-basis-appointment/no-basis-group</t>
+    <t>http://example.org/StructureDefinition/no-basis-group</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-27T14:52:10+02:00</t>
+    <t>2023-07-20T11:38:03+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,7 +87,7 @@
     <t>FHIR Version</t>
   </si>
   <si>
-    <t>4.3.0</t>
+    <t>4.0.1</t>
   </si>
   <si>
     <t>Kind</t>
@@ -124,117 +124,6 @@
   </si>
   <si>
     <t>element:Appointment</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>Slice Name</t>
-  </si>
-  <si>
-    <t>Alias(s)</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Must Support?</t>
-  </si>
-  <si>
-    <t>Is Modifier?</t>
-  </si>
-  <si>
-    <t>Is Summary?</t>
-  </si>
-  <si>
-    <t>Type(s)</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Requirements</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Meaning When Missing</t>
-  </si>
-  <si>
-    <t>Fixed Value</t>
-  </si>
-  <si>
-    <t>Pattern</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
-    <t>Maximum Length</t>
-  </si>
-  <si>
-    <t>Binding Strength</t>
-  </si>
-  <si>
-    <t>Binding Description</t>
-  </si>
-  <si>
-    <t>Binding Value Set</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Slicing Discriminator</t>
-  </si>
-  <si>
-    <t>Slicing Description</t>
-  </si>
-  <si>
-    <t>Slicing Ordered</t>
-  </si>
-  <si>
-    <t>Slicing Rules</t>
-  </si>
-  <si>
-    <t>Base Path</t>
-  </si>
-  <si>
-    <t>Base Min</t>
-  </si>
-  <si>
-    <t>Base Max</t>
-  </si>
-  <si>
-    <t>Condition(s)</t>
-  </si>
-  <si>
-    <t>Constraint(s)</t>
-  </si>
-  <si>
-    <t>Mapping: RIM Mapping</t>
   </si>
   <si>
     <t/>
@@ -260,7 +149,7 @@
     <t>Extension.id</t>
   </si>
   <si>
-    <t xml:space="preserve">id
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -329,7 +218,7 @@
 </t>
   </si>
   <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4B/extensibility.html) for a list).</t>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
   </si>
   <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
@@ -455,10 +344,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -638,7 +527,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK6"/>
+  <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -649,670 +538,555 @@
   <cols>
     <col min="1" max="1" width="19.00390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.00390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="7.68359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="1.0390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="6" max="6" width="2.15234375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="2.15234375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="1.0390625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="9.734375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.91015625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="17.07421875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="9.546875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="30" max="30" width="1.0390625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="5.60546875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="17.7265625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="33" max="33" width="2.15234375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="2.15234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" hidden="true" width="8.0" customWidth="false"/>
+    <col min="17" max="17" width="20.703125" customWidth="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="22.67578125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="4.58203125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s" s="1">
+      <c r="A1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" t="s" s="2">
         <v>38</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="G1" t="s" s="2">
         <v>39</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="H1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="L1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF1" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="AG1" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AH1" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="AI1" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="G1" t="s" s="1">
-        <v>43</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>44</v>
-      </c>
-      <c r="I1" t="s" s="1">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s" s="1">
-        <v>46</v>
-      </c>
-      <c r="K1" t="s" s="1">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s" s="1">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s" s="1">
-        <v>49</v>
-      </c>
-      <c r="N1" t="s" s="1">
-        <v>50</v>
-      </c>
-      <c r="O1" t="s" s="1">
-        <v>51</v>
-      </c>
-      <c r="P1" t="s" s="1">
-        <v>52</v>
-      </c>
-      <c r="Q1" t="s" s="1">
-        <v>53</v>
-      </c>
-      <c r="R1" t="s" s="1">
-        <v>54</v>
-      </c>
-      <c r="S1" t="s" s="1">
-        <v>55</v>
-      </c>
-      <c r="T1" t="s" s="1">
-        <v>56</v>
-      </c>
-      <c r="U1" t="s" s="1">
-        <v>57</v>
-      </c>
-      <c r="V1" t="s" s="1">
-        <v>58</v>
-      </c>
-      <c r="W1" t="s" s="1">
-        <v>59</v>
-      </c>
-      <c r="X1" t="s" s="1">
-        <v>60</v>
-      </c>
-      <c r="Y1" t="s" s="1">
-        <v>61</v>
-      </c>
-      <c r="Z1" t="s" s="1">
-        <v>62</v>
-      </c>
-      <c r="AA1" t="s" s="1">
-        <v>63</v>
-      </c>
-      <c r="AB1" t="s" s="1">
-        <v>64</v>
-      </c>
-      <c r="AC1" t="s" s="1">
-        <v>65</v>
-      </c>
-      <c r="AD1" t="s" s="1">
-        <v>66</v>
-      </c>
-      <c r="AE1" t="s" s="1">
-        <v>67</v>
-      </c>
-      <c r="AF1" t="s" s="1">
-        <v>68</v>
-      </c>
-      <c r="AG1" t="s" s="1">
-        <v>69</v>
-      </c>
-      <c r="AH1" t="s" s="1">
-        <v>70</v>
-      </c>
-      <c r="AI1" t="s" s="1">
-        <v>71</v>
-      </c>
-      <c r="AJ1" t="s" s="1">
-        <v>72</v>
-      </c>
-      <c r="AK1" t="s" s="1">
-        <v>73</v>
+      <c r="AJ1" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AK1" t="s" s="2">
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" t="s" s="2">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="AG2" t="s" s="2">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="N4" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="N4" t="s" s="2">
+        <v>61</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="N5" t="s" s="2">
-        <v>98</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="I6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="K6" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="S6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="T6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="U6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="V6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="W6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="X6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Z6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AA6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF6" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="AG6" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH6" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI6" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ6" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="AK6" t="s" s="2">
-        <v>99</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>